<commit_message>
constructor test cases completed
</commit_message>
<xml_diff>
--- a/testcases-doc/recipe-logic-test.xlsx
+++ b/testcases-doc/recipe-logic-test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zonyyu/Library/Mobile Documents/com~apple~CloudDocs/Documents/University Courses/CMPUT 301/shell379/testcases-doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EC136677-706D-EC43-8EE9-778AA9B867B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF1431E-02B6-2B41-A032-33E691E0F0B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{98FCFAA9-82C0-1540-A44E-DB917DB4D359}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="17">
   <si>
     <t>ID</t>
   </si>
@@ -71,12 +71,6 @@
     <t>&gt; 0</t>
   </si>
   <si>
-    <t>&lt;=0</t>
-  </si>
-  <si>
-    <t>len &lt;= 0</t>
-  </si>
-  <si>
     <t>image</t>
   </si>
   <si>
@@ -87,6 +81,12 @@
   </si>
   <si>
     <t>len = 0</t>
+  </si>
+  <si>
+    <t>equals(0)</t>
+  </si>
+  <si>
+    <t>&lt; 0</t>
   </si>
 </sst>
 </file>
@@ -158,14 +158,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -484,7 +483,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:B21"/>
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -512,7 +511,7 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -535,7 +534,7 @@
         <v>8</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -543,7 +542,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>10</v>
@@ -558,7 +557,7 @@
         <v>8</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -569,7 +568,7 @@
         <v>9</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>10</v>
@@ -581,7 +580,30 @@
         <v>8</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -595,62 +617,85 @@
         <v>10</v>
       </c>
       <c r="D6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
+        <v>6</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="6">
+        <v>7</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="6" t="s">
         <v>11</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="5">
-        <v>5</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="7">
-        <v>6</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -674,7 +719,7 @@
         <v>2</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -682,7 +727,7 @@
         <v>3</v>
       </c>
       <c r="B15">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -703,7 +748,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -711,7 +756,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
handled null string case
</commit_message>
<xml_diff>
--- a/testcases-doc/recipe-logic-test.xlsx
+++ b/testcases-doc/recipe-logic-test.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zonyyu/Library/Mobile Documents/com~apple~CloudDocs/Documents/University Courses/CMPUT 301/shell379/testcases-doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF1431E-02B6-2B41-A032-33E691E0F0B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BECBFDE-1842-1245-9FBF-8C0229E08549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{98FCFAA9-82C0-1540-A44E-DB917DB4D359}"/>
   </bookViews>
   <sheets>
     <sheet name="testConstructor" sheetId="1" r:id="rId1"/>
+    <sheet name="testGetterSetter" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="17">
   <si>
     <t>ID</t>
   </si>
@@ -480,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60A07BA4-1FCA-494A-8A07-86AD6F40AC0E}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+      <selection activeCell="Q26" sqref="Q26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -561,25 +562,25 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="3" t="s">
+      <c r="B4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>12</v>
       </c>
     </row>
@@ -591,41 +592,41 @@
         <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="4">
-        <v>4</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="4" t="s">
+      <c r="D6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>12</v>
       </c>
     </row>
@@ -640,126 +641,184 @@
         <v>10</v>
       </c>
       <c r="D7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="5">
-        <v>6</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
+        <v>7</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="6">
-        <v>7</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9" s="6" t="s">
+      <c r="F9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="5">
+        <v>8</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="6">
+        <v>9</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="6" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14">
-        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15">
-        <v>3</v>
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B16">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" t="s">
-        <v>8</v>
+        <v>2</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B18">
-        <v>2</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6C86AA2-8678-9349-9748-8897E931FE0D}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added more getter setter cases. Now on setComments
</commit_message>
<xml_diff>
--- a/testcases-doc/recipe-logic-test.xlsx
+++ b/testcases-doc/recipe-logic-test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zonyyu/Library/Mobile Documents/com~apple~CloudDocs/Documents/University Courses/CMPUT 301/shell379/testcases-doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BECBFDE-1842-1245-9FBF-8C0229E08549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46050685-18C4-E44C-BC0F-B378EEC63008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{98FCFAA9-82C0-1540-A44E-DB917DB4D359}"/>
+    <workbookView xWindow="3120" yWindow="2160" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{98FCFAA9-82C0-1540-A44E-DB917DB4D359}"/>
   </bookViews>
   <sheets>
     <sheet name="testConstructor" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="30">
   <si>
     <t>ID</t>
   </si>
@@ -88,14 +88,61 @@
   </si>
   <si>
     <t>&lt; 0</t>
+  </si>
+  <si>
+    <t>function name</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>params</t>
+  </si>
+  <si>
+    <t>Expected Results</t>
+  </si>
+  <si>
+    <t>setTitle</t>
+  </si>
+  <si>
+    <t>""</t>
+  </si>
+  <si>
+    <t>"valid title"</t>
+  </si>
+  <si>
+    <t>IllegalArgumentException</t>
+  </si>
+  <si>
+    <t>No Action</t>
+  </si>
+  <si>
+    <t>setPreparationTime</t>
+  </si>
+  <si>
+    <t>setServings</t>
+  </si>
+  <si>
+    <t>setCategory</t>
+  </si>
+  <si>
+    <t>"valid cat"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -159,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -167,6 +214,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,7 +531,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60A07BA4-1FCA-494A-8A07-86AD6F40AC0E}">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q26" sqref="Q26"/>
     </sheetView>
   </sheetViews>
@@ -813,12 +861,210 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6C86AA2-8678-9349-9748-8897E931FE0D}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q27" sqref="Q27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="23.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="7"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3">
+        <v>2</v>
+      </c>
+      <c r="C7" s="3">
+        <v>-1</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0</v>
+      </c>
+      <c r="C8" s="4">
+        <v>1</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4">
+        <v>1</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4">
+        <v>2</v>
+      </c>
+      <c r="C10" s="4">
+        <v>-1</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="5">
+        <v>0</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5">
+        <v>1</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5">
+        <v>2</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="5"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>